<commit_message>
Working version for just pipeline
</commit_message>
<xml_diff>
--- a/Fake-Salesforce-Clients.xlsx
+++ b/Fake-Salesforce-Clients.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15220" tabRatio="500"/>
+    <workbookView xWindow="-10760" yWindow="-19920" windowWidth="28160" windowHeight="15220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>OppID</t>
   </si>
@@ -54,13 +54,22 @@
   </si>
   <si>
     <t>Celgene</t>
+  </si>
+  <si>
+    <t>SS_Email</t>
+  </si>
+  <si>
+    <t>tallen@mdsol.com</t>
+  </si>
+  <si>
+    <t>WCT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +81,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,14 +111,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -377,18 +398,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -398,52 +420,88 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>55555555</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>123456789</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>234567890</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>234567890</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>444123453</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>6</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>890765432</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>